<commit_message>
added jhansi details to the xl
</commit_message>
<xml_diff>
--- a/abhi.xlsx
+++ b/abhi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2322391_cognizant_com/Documents/git/home/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC1048A8899C4D825BDE5903" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FD0E16B-A207-4D27-85B7-9DBC07DC9657}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC1048A8899C4D825BDE5903" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A05FF2BD-7ED1-4E5F-A6FC-8B100B8E4121}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Abhishek</t>
+  </si>
+  <si>
+    <t>Jhansi</t>
   </si>
 </sst>
 </file>
@@ -89,6 +92,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -387,6 +394,17 @@
         <v>9876543210</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>8874543985</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>